<commit_message>
Added option for user to enter name instead of id
</commit_message>
<xml_diff>
--- a/project/faculty_metrics.xlsx
+++ b/project/faculty_metrics.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{92E00D24-6F19-41F9-B851-31EC12858671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F74CDF3-1379-479B-9FEA-A79D13FC8215}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABF012AB-602A-4642-A3AD-8BA3B8EE6DF8}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="11856" xr2:uid="{ABF012AB-602A-4642-A3AD-8BA3B8EE6DF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,6 +587,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -888,9 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EB2196-06C4-46B3-A825-39D2CBADA2AB}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>